<commit_message>
Fixing names / scientific names
</commit_message>
<xml_diff>
--- a/forms/Form-1DR.xlsx
+++ b/forms/Form-1DR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\R libs\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329441FC-A6F3-45EE-AEF1-A550A10C5BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FA1691-CC29-499E-A18B-D5E62420A5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="5O4euoXp3wZfikUhVbwGMfw3acpHwF0QGHqLGhqkSE4QfnoccY7VPEsDDzzEBP5NB49UT+XbcZf1lZQTbDpLFA==" workbookSaltValue="DtEOIJKZ9UKP8oWrD+QpRw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -240,9 +240,6 @@
     <t>Bullet tuna</t>
   </si>
   <si>
-    <t>Narrow barred Spanish mackerel</t>
-  </si>
-  <si>
     <t>Indo-Pacific king mackerel</t>
   </si>
   <si>
@@ -342,12 +339,6 @@
     <t>Makaira nigricans</t>
   </si>
   <si>
-    <t>Makaira indica</t>
-  </si>
-  <si>
-    <t>Tetrapturus audax</t>
-  </si>
-  <si>
     <t>Istiophorus platypterus</t>
   </si>
   <si>
@@ -439,6 +430,15 @@
   </si>
   <si>
     <t>Porbeagle</t>
+  </si>
+  <si>
+    <t>Narrow-barred Spanish mackerel</t>
+  </si>
+  <si>
+    <t>Istiompax indica</t>
+  </si>
+  <si>
+    <t>Kajikia audax</t>
   </si>
 </sst>
 </file>
@@ -1081,27 +1081,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1111,18 +1102,12 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1132,9 +1117,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1205,9 +1187,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -1311,6 +1290,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1662,24 +1662,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="83"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="76"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="84"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="86"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="79"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="20"/>
@@ -1729,15 +1729,15 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
-      <c r="C8" s="80" t="s">
+      <c r="C8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="80"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="13"/>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="80"/>
+      <c r="G8" s="73"/>
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1848,7 +1848,7 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
-      <c r="C19" s="72" t="s">
+      <c r="C19" s="65" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="5"/>
@@ -1859,7 +1859,7 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
-      <c r="C20" s="73" t="s">
+      <c r="C20" s="66" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="5"/>
@@ -1908,11 +1908,11 @@
     </row>
     <row r="25" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="78"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="79"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="72"/>
       <c r="H25" s="9"/>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1970,88 +1970,88 @@
   <sheetData>
     <row r="1" spans="1:19" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="82"/>
-      <c r="O2" s="82"/>
-      <c r="P2" s="82"/>
-      <c r="Q2" s="82"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="83"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="76"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="99"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
-      <c r="L3" s="100"/>
-      <c r="M3" s="100"/>
-      <c r="N3" s="100"/>
-      <c r="O3" s="100"/>
-      <c r="P3" s="100"/>
-      <c r="Q3" s="100"/>
-      <c r="R3" s="100"/>
-      <c r="S3" s="101"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="93"/>
+      <c r="S3" s="94"/>
     </row>
     <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26"/>
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="102" t="s">
+      <c r="C4" s="89"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="95" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" s="96"/>
+      <c r="H4" s="95" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="96"/>
+      <c r="J4" s="95" t="s">
+        <v>124</v>
+      </c>
+      <c r="K4" s="96"/>
+      <c r="L4" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="G4" s="103"/>
-      <c r="H4" s="102" t="s">
+      <c r="M4" s="96"/>
+      <c r="N4" s="95" t="s">
+        <v>129</v>
+      </c>
+      <c r="O4" s="96"/>
+      <c r="P4" s="95" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q4" s="96"/>
+      <c r="R4" s="97" t="s">
         <v>123</v>
       </c>
-      <c r="I4" s="103"/>
-      <c r="J4" s="102" t="s">
-        <v>127</v>
-      </c>
-      <c r="K4" s="103"/>
-      <c r="L4" s="102" t="s">
-        <v>124</v>
-      </c>
-      <c r="M4" s="103"/>
-      <c r="N4" s="102" t="s">
-        <v>132</v>
-      </c>
-      <c r="O4" s="103"/>
-      <c r="P4" s="102" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q4" s="103"/>
-      <c r="R4" s="104" t="s">
-        <v>126</v>
-      </c>
-      <c r="S4" s="103"/>
+      <c r="S4" s="96"/>
     </row>
     <row r="5" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="27" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>20</v>
@@ -2062,51 +2062,51 @@
       <c r="E5" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="74" t="s">
-        <v>131</v>
-      </c>
-      <c r="G5" s="75" t="s">
-        <v>122</v>
-      </c>
-      <c r="H5" s="74" t="s">
-        <v>131</v>
-      </c>
-      <c r="I5" s="75" t="s">
-        <v>122</v>
-      </c>
-      <c r="J5" s="74" t="s">
-        <v>131</v>
-      </c>
-      <c r="K5" s="75" t="s">
-        <v>122</v>
-      </c>
-      <c r="L5" s="74" t="s">
-        <v>131</v>
-      </c>
-      <c r="M5" s="75" t="s">
-        <v>122</v>
-      </c>
-      <c r="N5" s="74" t="s">
-        <v>131</v>
-      </c>
-      <c r="O5" s="75" t="s">
-        <v>122</v>
-      </c>
-      <c r="P5" s="74" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q5" s="75" t="s">
-        <v>122</v>
-      </c>
-      <c r="R5" s="76" t="s">
-        <v>131</v>
-      </c>
-      <c r="S5" s="75" t="s">
-        <v>122</v>
+      <c r="F5" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="I5" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="J5" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="K5" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="L5" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="M5" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="N5" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="O5" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="P5" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q5" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="R5" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="S5" s="68" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="92" t="s">
+      <c r="B6" s="85" t="s">
         <v>54</v>
       </c>
       <c r="C6" s="31" t="s">
@@ -2115,52 +2115,52 @@
       <c r="D6" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="98" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="45"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="47"/>
+      <c r="S6" s="46"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="87"/>
+      <c r="C7" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="51"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="52"/>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="52"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="52"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="94"/>
-      <c r="C7" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" s="54"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="55"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="55"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="55"/>
-      <c r="R7" s="56"/>
-      <c r="S7" s="55"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="49"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="87" t="s">
+      <c r="B8" s="80" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="31" t="s">
@@ -2169,79 +2169,79 @@
       <c r="D8" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="98" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="45"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="46"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="47"/>
+      <c r="S8" s="46"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="81"/>
+      <c r="C9" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="100" t="s">
         <v>91</v>
       </c>
-      <c r="F8" s="51"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="52"/>
-      <c r="N8" s="51"/>
-      <c r="O8" s="52"/>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="52"/>
-      <c r="R8" s="53"/>
-      <c r="S8" s="52"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="88"/>
-      <c r="C9" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="39" t="s">
+      <c r="F9" s="51"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="53"/>
+      <c r="S9" s="52"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="82"/>
+      <c r="C10" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="99" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="57"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="57"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="57"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="57"/>
-      <c r="Q9" s="58"/>
-      <c r="R9" s="59"/>
-      <c r="S9" s="58"/>
-    </row>
-    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="89"/>
-      <c r="C10" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="54"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="54"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="55"/>
-      <c r="P10" s="54"/>
-      <c r="Q10" s="55"/>
-      <c r="R10" s="56"/>
-      <c r="S10" s="55"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="50"/>
+      <c r="S10" s="49"/>
     </row>
     <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="92" t="s">
-        <v>129</v>
+      <c r="B11" s="85" t="s">
+        <v>126</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>30</v>
@@ -2249,708 +2249,708 @@
       <c r="D11" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="98" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="45"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="46"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="46"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="86"/>
+      <c r="C12" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="100" t="s">
         <v>94</v>
       </c>
-      <c r="F11" s="51"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="52"/>
-      <c r="P11" s="51"/>
-      <c r="Q11" s="52"/>
-      <c r="R11" s="53"/>
-      <c r="S11" s="52"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="93"/>
-      <c r="C12" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="39" t="s">
+      <c r="F12" s="51"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="52"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="52"/>
+      <c r="R12" s="53"/>
+      <c r="S12" s="52"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="86"/>
+      <c r="C13" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="F12" s="57"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="57"/>
-      <c r="Q12" s="58"/>
-      <c r="R12" s="59"/>
-      <c r="S12" s="58"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="93"/>
-      <c r="C13" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="39" t="s">
+      <c r="F13" s="51"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="52"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="52"/>
+      <c r="R13" s="53"/>
+      <c r="S13" s="52"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="87"/>
+      <c r="C14" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="99" t="s">
         <v>96</v>
       </c>
-      <c r="F13" s="57"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="57"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="57"/>
-      <c r="Q13" s="58"/>
-      <c r="R13" s="59"/>
-      <c r="S13" s="58"/>
-    </row>
-    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="94"/>
-      <c r="C14" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="36" t="s">
+      <c r="F14" s="48"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="50"/>
+      <c r="S14" s="49"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="86" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="64" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" s="101" t="s">
         <v>97</v>
       </c>
-      <c r="F14" s="54"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="55"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="55"/>
-      <c r="P14" s="54"/>
-      <c r="Q14" s="55"/>
-      <c r="R14" s="56"/>
-      <c r="S14" s="55"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="93" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="70" t="s">
+      <c r="F15" s="56"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="57"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="56"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="58"/>
+      <c r="S15" s="57"/>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="87"/>
+      <c r="C16" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="71" t="s">
+      <c r="E16" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="F15" s="62"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="63"/>
-      <c r="L15" s="62"/>
-      <c r="M15" s="63"/>
-      <c r="N15" s="62"/>
-      <c r="O15" s="63"/>
-      <c r="P15" s="62"/>
-      <c r="Q15" s="63"/>
-      <c r="R15" s="64"/>
-      <c r="S15" s="63"/>
-    </row>
-    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="94"/>
-      <c r="C16" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="F16" s="54"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="55"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="55"/>
-      <c r="P16" s="54"/>
-      <c r="Q16" s="55"/>
-      <c r="R16" s="56"/>
-      <c r="S16" s="55"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="48"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="48"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="50"/>
+      <c r="S16" s="49"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="80" t="s">
         <v>56</v>
       </c>
       <c r="C17" s="31" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="98" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="45"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="46"/>
+      <c r="R17" s="47"/>
+      <c r="S17" s="46"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B18" s="81"/>
+      <c r="C18" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E18" s="100" t="s">
+        <v>132</v>
+      </c>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="52"/>
+      <c r="N18" s="51"/>
+      <c r="O18" s="52"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="52"/>
+      <c r="R18" s="53"/>
+      <c r="S18" s="52"/>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B19" s="81"/>
+      <c r="C19" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="100" t="s">
+        <v>133</v>
+      </c>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="52"/>
+      <c r="R19" s="53"/>
+      <c r="S19" s="52"/>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B20" s="81"/>
+      <c r="C20" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="100" t="s">
         <v>100</v>
       </c>
-      <c r="F17" s="51"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="51"/>
-      <c r="O17" s="52"/>
-      <c r="P17" s="51"/>
-      <c r="Q17" s="52"/>
-      <c r="R17" s="53"/>
-      <c r="S17" s="52"/>
-    </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="88"/>
-      <c r="C18" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="39" t="s">
+      <c r="F20" s="51"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="52"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="52"/>
+      <c r="P20" s="51"/>
+      <c r="Q20" s="52"/>
+      <c r="R20" s="53"/>
+      <c r="S20" s="52"/>
+    </row>
+    <row r="21" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="82"/>
+      <c r="C21" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="99" t="s">
         <v>101</v>
       </c>
-      <c r="F18" s="57"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="58"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="58"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="58"/>
-      <c r="P18" s="57"/>
-      <c r="Q18" s="58"/>
-      <c r="R18" s="59"/>
-      <c r="S18" s="58"/>
-    </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="88"/>
-      <c r="C19" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="E19" s="39" t="s">
+      <c r="F21" s="48"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="49"/>
+      <c r="P21" s="48"/>
+      <c r="Q21" s="49"/>
+      <c r="R21" s="50"/>
+      <c r="S21" s="49"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B22" s="83" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="102" t="s">
         <v>102</v>
       </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="58"/>
-      <c r="L19" s="57"/>
-      <c r="M19" s="58"/>
-      <c r="N19" s="57"/>
-      <c r="O19" s="58"/>
-      <c r="P19" s="57"/>
-      <c r="Q19" s="58"/>
-      <c r="R19" s="59"/>
-      <c r="S19" s="58"/>
-    </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="88"/>
-      <c r="C20" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="E20" s="39" t="s">
+      <c r="F22" s="54"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="55"/>
+      <c r="P22" s="56"/>
+      <c r="Q22" s="57"/>
+      <c r="R22" s="58"/>
+      <c r="S22" s="57"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="83"/>
+      <c r="C23" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="F20" s="57"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="58"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="58"/>
-      <c r="P20" s="57"/>
-      <c r="Q20" s="58"/>
-      <c r="R20" s="59"/>
-      <c r="S20" s="58"/>
-    </row>
-    <row r="21" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="89"/>
-      <c r="C21" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="36" t="s">
+      <c r="F23" s="59"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="59"/>
+      <c r="O23" s="60"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="52"/>
+      <c r="R23" s="53"/>
+      <c r="S23" s="52"/>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="83"/>
+      <c r="C24" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="103" t="s">
         <v>104</v>
       </c>
-      <c r="F21" s="54"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="55"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="54"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="54"/>
-      <c r="Q21" s="55"/>
-      <c r="R21" s="56"/>
-      <c r="S21" s="55"/>
-    </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="90" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="E22" s="43" t="s">
+      <c r="F24" s="59"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="59"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="59"/>
+      <c r="O24" s="60"/>
+      <c r="P24" s="51"/>
+      <c r="Q24" s="52"/>
+      <c r="R24" s="53"/>
+      <c r="S24" s="52"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="83"/>
+      <c r="C25" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="E25" s="103" t="s">
         <v>105</v>
       </c>
-      <c r="F22" s="60"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="60"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="62"/>
-      <c r="K22" s="63"/>
-      <c r="L22" s="60"/>
-      <c r="M22" s="61"/>
-      <c r="N22" s="60"/>
-      <c r="O22" s="61"/>
-      <c r="P22" s="62"/>
-      <c r="Q22" s="63"/>
-      <c r="R22" s="64"/>
-      <c r="S22" s="63"/>
-    </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="90"/>
-      <c r="C23" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23" s="46" t="s">
+      <c r="F25" s="59"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="59"/>
+      <c r="M25" s="60"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="60"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="52"/>
+      <c r="R25" s="53"/>
+      <c r="S25" s="52"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="83"/>
+      <c r="C26" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="103" t="s">
         <v>106</v>
       </c>
-      <c r="F23" s="65"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="58"/>
-      <c r="L23" s="65"/>
-      <c r="M23" s="66"/>
-      <c r="N23" s="65"/>
-      <c r="O23" s="66"/>
-      <c r="P23" s="57"/>
-      <c r="Q23" s="58"/>
-      <c r="R23" s="59"/>
-      <c r="S23" s="58"/>
-    </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B24" s="90"/>
-      <c r="C24" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="46" t="s">
+      <c r="F26" s="59"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="59"/>
+      <c r="M26" s="60"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="60"/>
+      <c r="P26" s="51"/>
+      <c r="Q26" s="52"/>
+      <c r="R26" s="53"/>
+      <c r="S26" s="52"/>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="83"/>
+      <c r="C27" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="103" t="s">
         <v>107</v>
       </c>
-      <c r="F24" s="65"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="58"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="66"/>
-      <c r="N24" s="65"/>
-      <c r="O24" s="66"/>
-      <c r="P24" s="57"/>
-      <c r="Q24" s="58"/>
-      <c r="R24" s="59"/>
-      <c r="S24" s="58"/>
-    </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="90"/>
-      <c r="C25" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="45" t="s">
-        <v>133</v>
-      </c>
-      <c r="E25" s="46" t="s">
+      <c r="F27" s="59"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="51"/>
+      <c r="M27" s="52"/>
+      <c r="N27" s="59"/>
+      <c r="O27" s="60"/>
+      <c r="P27" s="51"/>
+      <c r="Q27" s="52"/>
+      <c r="R27" s="53"/>
+      <c r="S27" s="52"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="83"/>
+      <c r="C28" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="103" t="s">
         <v>108</v>
       </c>
-      <c r="F25" s="65"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="66"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="65"/>
-      <c r="M25" s="66"/>
-      <c r="N25" s="65"/>
-      <c r="O25" s="66"/>
-      <c r="P25" s="57"/>
-      <c r="Q25" s="58"/>
-      <c r="R25" s="59"/>
-      <c r="S25" s="58"/>
-    </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="90"/>
-      <c r="C26" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="46" t="s">
+      <c r="F28" s="51"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="51"/>
+      <c r="M28" s="52"/>
+      <c r="N28" s="51"/>
+      <c r="O28" s="52"/>
+      <c r="P28" s="51"/>
+      <c r="Q28" s="52"/>
+      <c r="R28" s="53"/>
+      <c r="S28" s="52"/>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B29" s="83"/>
+      <c r="C29" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="103" t="s">
         <v>109</v>
       </c>
-      <c r="F26" s="65"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="66"/>
-      <c r="J26" s="57"/>
-      <c r="K26" s="58"/>
-      <c r="L26" s="65"/>
-      <c r="M26" s="66"/>
-      <c r="N26" s="65"/>
-      <c r="O26" s="66"/>
-      <c r="P26" s="57"/>
-      <c r="Q26" s="58"/>
-      <c r="R26" s="59"/>
-      <c r="S26" s="58"/>
-    </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="90"/>
-      <c r="C27" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="E27" s="46" t="s">
+      <c r="F29" s="51"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="51"/>
+      <c r="M29" s="52"/>
+      <c r="N29" s="51"/>
+      <c r="O29" s="52"/>
+      <c r="P29" s="51"/>
+      <c r="Q29" s="52"/>
+      <c r="R29" s="53"/>
+      <c r="S29" s="52"/>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B30" s="83"/>
+      <c r="C30" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="103" t="s">
         <v>110</v>
       </c>
-      <c r="F27" s="65"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="66"/>
-      <c r="J27" s="57"/>
-      <c r="K27" s="58"/>
-      <c r="L27" s="57"/>
-      <c r="M27" s="58"/>
-      <c r="N27" s="65"/>
-      <c r="O27" s="66"/>
-      <c r="P27" s="57"/>
-      <c r="Q27" s="58"/>
-      <c r="R27" s="59"/>
-      <c r="S27" s="58"/>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="90"/>
-      <c r="C28" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="E28" s="46" t="s">
+      <c r="F30" s="59"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="52"/>
+      <c r="L30" s="51"/>
+      <c r="M30" s="52"/>
+      <c r="N30" s="59"/>
+      <c r="O30" s="60"/>
+      <c r="P30" s="51"/>
+      <c r="Q30" s="52"/>
+      <c r="R30" s="53"/>
+      <c r="S30" s="52"/>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B31" s="83"/>
+      <c r="C31" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="103" t="s">
         <v>111</v>
       </c>
-      <c r="F28" s="57"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="58"/>
-      <c r="L28" s="57"/>
-      <c r="M28" s="58"/>
-      <c r="N28" s="57"/>
-      <c r="O28" s="58"/>
-      <c r="P28" s="57"/>
-      <c r="Q28" s="58"/>
-      <c r="R28" s="59"/>
-      <c r="S28" s="58"/>
-    </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="90"/>
-      <c r="C29" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" s="46" t="s">
+      <c r="F31" s="59"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="51"/>
+      <c r="M31" s="52"/>
+      <c r="N31" s="59"/>
+      <c r="O31" s="60"/>
+      <c r="P31" s="51"/>
+      <c r="Q31" s="52"/>
+      <c r="R31" s="53"/>
+      <c r="S31" s="52"/>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B32" s="83"/>
+      <c r="C32" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="F29" s="57"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="57"/>
-      <c r="K29" s="58"/>
-      <c r="L29" s="57"/>
-      <c r="M29" s="58"/>
-      <c r="N29" s="57"/>
-      <c r="O29" s="58"/>
-      <c r="P29" s="57"/>
-      <c r="Q29" s="58"/>
-      <c r="R29" s="59"/>
-      <c r="S29" s="58"/>
-    </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="90"/>
-      <c r="C30" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="E30" s="46" t="s">
+      <c r="F32" s="59"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="52"/>
+      <c r="L32" s="59"/>
+      <c r="M32" s="60"/>
+      <c r="N32" s="59"/>
+      <c r="O32" s="60"/>
+      <c r="P32" s="51"/>
+      <c r="Q32" s="52"/>
+      <c r="R32" s="53"/>
+      <c r="S32" s="52"/>
+    </row>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B33" s="83"/>
+      <c r="C33" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" s="103" t="s">
         <v>113</v>
       </c>
-      <c r="F30" s="65"/>
-      <c r="G30" s="66"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="66"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="58"/>
-      <c r="L30" s="57"/>
-      <c r="M30" s="58"/>
-      <c r="N30" s="65"/>
-      <c r="O30" s="66"/>
-      <c r="P30" s="57"/>
-      <c r="Q30" s="58"/>
-      <c r="R30" s="59"/>
-      <c r="S30" s="58"/>
-    </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="90"/>
-      <c r="C31" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D31" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" s="46" t="s">
+      <c r="F33" s="59"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="52"/>
+      <c r="L33" s="59"/>
+      <c r="M33" s="60"/>
+      <c r="N33" s="59"/>
+      <c r="O33" s="60"/>
+      <c r="P33" s="51"/>
+      <c r="Q33" s="52"/>
+      <c r="R33" s="53"/>
+      <c r="S33" s="52"/>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B34" s="83"/>
+      <c r="C34" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" s="103" t="s">
         <v>114</v>
       </c>
-      <c r="F31" s="65"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="66"/>
-      <c r="J31" s="57"/>
-      <c r="K31" s="58"/>
-      <c r="L31" s="57"/>
-      <c r="M31" s="58"/>
-      <c r="N31" s="65"/>
-      <c r="O31" s="66"/>
-      <c r="P31" s="57"/>
-      <c r="Q31" s="58"/>
-      <c r="R31" s="59"/>
-      <c r="S31" s="58"/>
-    </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="90"/>
-      <c r="C32" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="D32" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="E32" s="46" t="s">
+      <c r="F34" s="59"/>
+      <c r="G34" s="60"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="52"/>
+      <c r="L34" s="59"/>
+      <c r="M34" s="60"/>
+      <c r="N34" s="59"/>
+      <c r="O34" s="60"/>
+      <c r="P34" s="51"/>
+      <c r="Q34" s="52"/>
+      <c r="R34" s="53"/>
+      <c r="S34" s="52"/>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B35" s="83"/>
+      <c r="C35" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" s="103" t="s">
         <v>115</v>
       </c>
-      <c r="F32" s="65"/>
-      <c r="G32" s="66"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="66"/>
-      <c r="J32" s="57"/>
-      <c r="K32" s="58"/>
-      <c r="L32" s="65"/>
-      <c r="M32" s="66"/>
-      <c r="N32" s="65"/>
-      <c r="O32" s="66"/>
-      <c r="P32" s="57"/>
-      <c r="Q32" s="58"/>
-      <c r="R32" s="59"/>
-      <c r="S32" s="58"/>
-    </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B33" s="90"/>
-      <c r="C33" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="E33" s="46" t="s">
+      <c r="F35" s="59"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="59"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="52"/>
+      <c r="N35" s="59"/>
+      <c r="O35" s="60"/>
+      <c r="P35" s="51"/>
+      <c r="Q35" s="52"/>
+      <c r="R35" s="53"/>
+      <c r="S35" s="52"/>
+    </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B36" s="83"/>
+      <c r="C36" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" s="103" t="s">
         <v>116</v>
       </c>
-      <c r="F33" s="65"/>
-      <c r="G33" s="66"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="66"/>
-      <c r="J33" s="57"/>
-      <c r="K33" s="58"/>
-      <c r="L33" s="65"/>
-      <c r="M33" s="66"/>
-      <c r="N33" s="65"/>
-      <c r="O33" s="66"/>
-      <c r="P33" s="57"/>
-      <c r="Q33" s="58"/>
-      <c r="R33" s="59"/>
-      <c r="S33" s="58"/>
-    </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B34" s="90"/>
-      <c r="C34" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="E34" s="46" t="s">
+      <c r="F36" s="59"/>
+      <c r="G36" s="60"/>
+      <c r="H36" s="59"/>
+      <c r="I36" s="60"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="59"/>
+      <c r="M36" s="60"/>
+      <c r="N36" s="59"/>
+      <c r="O36" s="60"/>
+      <c r="P36" s="51"/>
+      <c r="Q36" s="52"/>
+      <c r="R36" s="53"/>
+      <c r="S36" s="52"/>
+    </row>
+    <row r="37" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="84"/>
+      <c r="C37" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37" s="104" t="s">
         <v>117</v>
       </c>
-      <c r="F34" s="65"/>
-      <c r="G34" s="66"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="66"/>
-      <c r="J34" s="57"/>
-      <c r="K34" s="58"/>
-      <c r="L34" s="65"/>
-      <c r="M34" s="66"/>
-      <c r="N34" s="65"/>
-      <c r="O34" s="66"/>
-      <c r="P34" s="57"/>
-      <c r="Q34" s="58"/>
-      <c r="R34" s="59"/>
-      <c r="S34" s="58"/>
-    </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B35" s="90"/>
-      <c r="C35" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="D35" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E35" s="46" t="s">
-        <v>118</v>
-      </c>
-      <c r="F35" s="65"/>
-      <c r="G35" s="66"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="66"/>
-      <c r="J35" s="57"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="57"/>
-      <c r="M35" s="58"/>
-      <c r="N35" s="65"/>
-      <c r="O35" s="66"/>
-      <c r="P35" s="57"/>
-      <c r="Q35" s="58"/>
-      <c r="R35" s="59"/>
-      <c r="S35" s="58"/>
-    </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B36" s="90"/>
-      <c r="C36" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="D36" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="E36" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="F36" s="65"/>
-      <c r="G36" s="66"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="66"/>
-      <c r="J36" s="57"/>
-      <c r="K36" s="58"/>
-      <c r="L36" s="65"/>
-      <c r="M36" s="66"/>
-      <c r="N36" s="65"/>
-      <c r="O36" s="66"/>
-      <c r="P36" s="57"/>
-      <c r="Q36" s="58"/>
-      <c r="R36" s="59"/>
-      <c r="S36" s="58"/>
-    </row>
-    <row r="37" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="91"/>
-      <c r="C37" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="D37" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="E37" s="50" t="s">
-        <v>120</v>
-      </c>
-      <c r="F37" s="67"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="67"/>
-      <c r="I37" s="68"/>
-      <c r="J37" s="54"/>
-      <c r="K37" s="55"/>
-      <c r="L37" s="67"/>
-      <c r="M37" s="68"/>
-      <c r="N37" s="67"/>
-      <c r="O37" s="68"/>
-      <c r="P37" s="54"/>
-      <c r="Q37" s="55"/>
-      <c r="R37" s="56"/>
-      <c r="S37" s="55"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="61"/>
+      <c r="I37" s="62"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="61"/>
+      <c r="M37" s="62"/>
+      <c r="N37" s="61"/>
+      <c r="O37" s="62"/>
+      <c r="P37" s="48"/>
+      <c r="Q37" s="49"/>
+      <c r="R37" s="50"/>
+      <c r="S37" s="49"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="kEALum4tqoAV/9u4KS7UyhwdscrzyDk46SeKygNA0R9pEhuRRoTpYewnIemEncQU8EASVi7d3SjiiBG5pU+i8w==" saltValue="sG6x8BrdodVItigIkf0RIg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="S1AOELBYt6/XOWTpFRCtaOTetcdUEQLpNxTcriTyQqR7MCbDkGBv0zTywWR1wQrjkN8mQJoTbNbjQqwEyUQd3g==" saltValue="nCuj8+GXpxALTSwhCjkizg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="B22:B37"/>

</xml_diff>

<commit_message>
Correction of "Pole and line" to "Pole-and-line" and "Troll lines" to "Trolling line" for consistency with the IOTC Data Reference Catalogue
</commit_message>
<xml_diff>
--- a/forms/Form-1DR.xlsx
+++ b/forms/Form-1DR.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\R libs\workflow\forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-workflow\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FA1691-CC29-499E-A18B-D5E62420A5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3846FC-C587-44FB-819E-6E3BB2ABCB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="5O4euoXp3wZfikUhVbwGMfw3acpHwF0QGHqLGhqkSE4QfnoccY7VPEsDDzzEBP5NB49UT+XbcZf1lZQTbDpLFA==" workbookSaltValue="DtEOIJKZ9UKP8oWrD+QpRw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -399,9 +399,6 @@
     <t>Industrial</t>
   </si>
   <si>
-    <t>PL - Pole and line</t>
-  </si>
-  <si>
     <t>PS - Purse seine</t>
   </si>
   <si>
@@ -426,9 +423,6 @@
     <t>Coastal</t>
   </si>
   <si>
-    <t>TL - Troll lines</t>
-  </si>
-  <si>
     <t>Porbeagle</t>
   </si>
   <si>
@@ -439,6 +433,12 @@
   </si>
   <si>
     <t>Kajikia audax</t>
+  </si>
+  <si>
+    <t>PL - Pole-and-line</t>
+  </si>
+  <si>
+    <t>TL - Trolling line</t>
   </si>
 </sst>
 </file>
@@ -1204,6 +1204,27 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1290,27 +1311,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1646,7 +1646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1662,24 +1662,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="76"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="83"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="77"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="79"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="86"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="20"/>
@@ -1729,15 +1729,15 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="73"/>
+      <c r="D8" s="80"/>
       <c r="E8" s="13"/>
-      <c r="F8" s="73" t="s">
+      <c r="F8" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="73"/>
+      <c r="G8" s="80"/>
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1908,11 +1908,11 @@
     </row>
     <row r="25" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
-      <c r="C25" s="70"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="72"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="78"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="79"/>
       <c r="H25" s="9"/>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1954,8 +1954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1970,88 +1970,88 @@
   <sheetData>
     <row r="1" spans="1:19" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="76"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="83"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="92"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="93"/>
-      <c r="S3" s="94"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="100"/>
+      <c r="R3" s="100"/>
+      <c r="S3" s="101"/>
     </row>
     <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26"/>
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="89"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="95" t="s">
+      <c r="C4" s="96"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="G4" s="96"/>
-      <c r="H4" s="95" t="s">
+      <c r="G4" s="103"/>
+      <c r="H4" s="102" t="s">
+        <v>132</v>
+      </c>
+      <c r="I4" s="103"/>
+      <c r="J4" s="102" t="s">
+        <v>123</v>
+      </c>
+      <c r="K4" s="103"/>
+      <c r="L4" s="102" t="s">
         <v>120</v>
       </c>
-      <c r="I4" s="96"/>
-      <c r="J4" s="95" t="s">
-        <v>124</v>
-      </c>
-      <c r="K4" s="96"/>
-      <c r="L4" s="95" t="s">
+      <c r="M4" s="103"/>
+      <c r="N4" s="102" t="s">
+        <v>133</v>
+      </c>
+      <c r="O4" s="103"/>
+      <c r="P4" s="102" t="s">
         <v>121</v>
       </c>
-      <c r="M4" s="96"/>
-      <c r="N4" s="95" t="s">
-        <v>129</v>
-      </c>
-      <c r="O4" s="96"/>
-      <c r="P4" s="95" t="s">
+      <c r="Q4" s="103"/>
+      <c r="R4" s="104" t="s">
         <v>122</v>
       </c>
-      <c r="Q4" s="96"/>
-      <c r="R4" s="97" t="s">
-        <v>123</v>
-      </c>
-      <c r="S4" s="96"/>
+      <c r="S4" s="103"/>
     </row>
     <row r="5" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>20</v>
@@ -2063,50 +2063,50 @@
         <v>21</v>
       </c>
       <c r="F5" s="67" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G5" s="68" t="s">
         <v>119</v>
       </c>
       <c r="H5" s="67" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I5" s="68" t="s">
         <v>119</v>
       </c>
       <c r="J5" s="67" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K5" s="68" t="s">
         <v>119</v>
       </c>
       <c r="L5" s="67" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M5" s="68" t="s">
         <v>119</v>
       </c>
       <c r="N5" s="67" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O5" s="68" t="s">
         <v>119</v>
       </c>
       <c r="P5" s="67" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Q5" s="68" t="s">
         <v>119</v>
       </c>
       <c r="R5" s="69" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="S5" s="68" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="92" t="s">
         <v>54</v>
       </c>
       <c r="C6" s="31" t="s">
@@ -2115,7 +2115,7 @@
       <c r="D6" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="98" t="s">
+      <c r="E6" s="70" t="s">
         <v>88</v>
       </c>
       <c r="F6" s="45"/>
@@ -2134,14 +2134,14 @@
       <c r="S6" s="46"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="87"/>
+      <c r="B7" s="94"/>
       <c r="C7" s="33" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="99" t="s">
+      <c r="E7" s="71" t="s">
         <v>89</v>
       </c>
       <c r="F7" s="48"/>
@@ -2160,7 +2160,7 @@
       <c r="S7" s="49"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="87" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="31" t="s">
@@ -2169,7 +2169,7 @@
       <c r="D8" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="98" t="s">
+      <c r="E8" s="70" t="s">
         <v>90</v>
       </c>
       <c r="F8" s="45"/>
@@ -2188,14 +2188,14 @@
       <c r="S8" s="46"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="81"/>
+      <c r="B9" s="88"/>
       <c r="C9" s="35" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="100" t="s">
+      <c r="E9" s="72" t="s">
         <v>91</v>
       </c>
       <c r="F9" s="51"/>
@@ -2214,14 +2214,14 @@
       <c r="S9" s="52"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="82"/>
+      <c r="B10" s="89"/>
       <c r="C10" s="33" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="99" t="s">
+      <c r="E10" s="71" t="s">
         <v>92</v>
       </c>
       <c r="F10" s="48"/>
@@ -2240,8 +2240,8 @@
       <c r="S10" s="49"/>
     </row>
     <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="85" t="s">
-        <v>126</v>
+      <c r="B11" s="92" t="s">
+        <v>125</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>30</v>
@@ -2249,7 +2249,7 @@
       <c r="D11" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="98" t="s">
+      <c r="E11" s="70" t="s">
         <v>93</v>
       </c>
       <c r="F11" s="45"/>
@@ -2268,14 +2268,14 @@
       <c r="S11" s="46"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="86"/>
+      <c r="B12" s="93"/>
       <c r="C12" s="35" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="100" t="s">
+      <c r="E12" s="72" t="s">
         <v>94</v>
       </c>
       <c r="F12" s="51"/>
@@ -2294,14 +2294,14 @@
       <c r="S12" s="52"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="86"/>
+      <c r="B13" s="93"/>
       <c r="C13" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="100" t="s">
+      <c r="E13" s="72" t="s">
         <v>95</v>
       </c>
       <c r="F13" s="51"/>
@@ -2320,14 +2320,14 @@
       <c r="S13" s="52"/>
     </row>
     <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="87"/>
+      <c r="B14" s="94"/>
       <c r="C14" s="33" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="99" t="s">
+      <c r="E14" s="71" t="s">
         <v>96</v>
       </c>
       <c r="F14" s="48"/>
@@ -2346,16 +2346,16 @@
       <c r="S14" s="49"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="86" t="s">
-        <v>127</v>
+      <c r="B15" s="93" t="s">
+        <v>126</v>
       </c>
       <c r="C15" s="63" t="s">
         <v>31</v>
       </c>
       <c r="D15" s="64" t="s">
-        <v>131</v>
-      </c>
-      <c r="E15" s="101" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="73" t="s">
         <v>97</v>
       </c>
       <c r="F15" s="56"/>
@@ -2374,14 +2374,14 @@
       <c r="S15" s="57"/>
     </row>
     <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="87"/>
+      <c r="B16" s="94"/>
       <c r="C16" s="33" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="99" t="s">
+      <c r="E16" s="71" t="s">
         <v>98</v>
       </c>
       <c r="F16" s="48"/>
@@ -2400,7 +2400,7 @@
       <c r="S16" s="49"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="80" t="s">
+      <c r="B17" s="87" t="s">
         <v>56</v>
       </c>
       <c r="C17" s="31" t="s">
@@ -2409,7 +2409,7 @@
       <c r="D17" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="98" t="s">
+      <c r="E17" s="70" t="s">
         <v>99</v>
       </c>
       <c r="F17" s="45"/>
@@ -2428,15 +2428,15 @@
       <c r="S17" s="46"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="81"/>
+      <c r="B18" s="88"/>
       <c r="C18" s="35" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="100" t="s">
-        <v>132</v>
+      <c r="E18" s="72" t="s">
+        <v>130</v>
       </c>
       <c r="F18" s="51"/>
       <c r="G18" s="52"/>
@@ -2454,15 +2454,15 @@
       <c r="S18" s="52"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="81"/>
+      <c r="B19" s="88"/>
       <c r="C19" s="35" t="s">
         <v>35</v>
       </c>
       <c r="D19" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="100" t="s">
-        <v>133</v>
+      <c r="E19" s="72" t="s">
+        <v>131</v>
       </c>
       <c r="F19" s="51"/>
       <c r="G19" s="52"/>
@@ -2480,14 +2480,14 @@
       <c r="S19" s="52"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="81"/>
+      <c r="B20" s="88"/>
       <c r="C20" s="35" t="s">
         <v>36</v>
       </c>
       <c r="D20" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="100" t="s">
+      <c r="E20" s="72" t="s">
         <v>100</v>
       </c>
       <c r="F20" s="51"/>
@@ -2506,14 +2506,14 @@
       <c r="S20" s="52"/>
     </row>
     <row r="21" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="82"/>
+      <c r="B21" s="89"/>
       <c r="C21" s="33" t="s">
         <v>37</v>
       </c>
       <c r="D21" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="99" t="s">
+      <c r="E21" s="71" t="s">
         <v>101</v>
       </c>
       <c r="F21" s="48"/>
@@ -2532,7 +2532,7 @@
       <c r="S21" s="49"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="83" t="s">
+      <c r="B22" s="90" t="s">
         <v>57</v>
       </c>
       <c r="C22" s="38" t="s">
@@ -2541,7 +2541,7 @@
       <c r="D22" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="102" t="s">
+      <c r="E22" s="74" t="s">
         <v>102</v>
       </c>
       <c r="F22" s="54"/>
@@ -2560,14 +2560,14 @@
       <c r="S22" s="57"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="83"/>
+      <c r="B23" s="90"/>
       <c r="C23" s="40" t="s">
         <v>39</v>
       </c>
       <c r="D23" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="103" t="s">
+      <c r="E23" s="75" t="s">
         <v>103</v>
       </c>
       <c r="F23" s="59"/>
@@ -2586,14 +2586,14 @@
       <c r="S23" s="52"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B24" s="83"/>
+      <c r="B24" s="90"/>
       <c r="C24" s="42" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="103" t="s">
+      <c r="E24" s="75" t="s">
         <v>104</v>
       </c>
       <c r="F24" s="59"/>
@@ -2612,14 +2612,14 @@
       <c r="S24" s="52"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="83"/>
+      <c r="B25" s="90"/>
       <c r="C25" s="40" t="s">
         <v>41</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="E25" s="103" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" s="75" t="s">
         <v>105</v>
       </c>
       <c r="F25" s="59"/>
@@ -2638,14 +2638,14 @@
       <c r="S25" s="52"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="83"/>
+      <c r="B26" s="90"/>
       <c r="C26" s="42" t="s">
         <v>42</v>
       </c>
       <c r="D26" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="103" t="s">
+      <c r="E26" s="75" t="s">
         <v>106</v>
       </c>
       <c r="F26" s="59"/>
@@ -2664,14 +2664,14 @@
       <c r="S26" s="52"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="83"/>
+      <c r="B27" s="90"/>
       <c r="C27" s="40" t="s">
         <v>43</v>
       </c>
       <c r="D27" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="103" t="s">
+      <c r="E27" s="75" t="s">
         <v>107</v>
       </c>
       <c r="F27" s="59"/>
@@ -2690,14 +2690,14 @@
       <c r="S27" s="52"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="83"/>
+      <c r="B28" s="90"/>
       <c r="C28" s="42" t="s">
         <v>44</v>
       </c>
       <c r="D28" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="103" t="s">
+      <c r="E28" s="75" t="s">
         <v>108</v>
       </c>
       <c r="F28" s="51"/>
@@ -2716,14 +2716,14 @@
       <c r="S28" s="52"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="83"/>
+      <c r="B29" s="90"/>
       <c r="C29" s="42" t="s">
         <v>45</v>
       </c>
       <c r="D29" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="103" t="s">
+      <c r="E29" s="75" t="s">
         <v>109</v>
       </c>
       <c r="F29" s="51"/>
@@ -2742,14 +2742,14 @@
       <c r="S29" s="52"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="83"/>
+      <c r="B30" s="90"/>
       <c r="C30" s="42" t="s">
         <v>46</v>
       </c>
       <c r="D30" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="E30" s="103" t="s">
+      <c r="E30" s="75" t="s">
         <v>110</v>
       </c>
       <c r="F30" s="59"/>
@@ -2768,14 +2768,14 @@
       <c r="S30" s="52"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="83"/>
+      <c r="B31" s="90"/>
       <c r="C31" s="40" t="s">
         <v>47</v>
       </c>
       <c r="D31" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="E31" s="103" t="s">
+      <c r="E31" s="75" t="s">
         <v>111</v>
       </c>
       <c r="F31" s="59"/>
@@ -2794,14 +2794,14 @@
       <c r="S31" s="52"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="83"/>
+      <c r="B32" s="90"/>
       <c r="C32" s="40" t="s">
         <v>48</v>
       </c>
       <c r="D32" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="E32" s="103" t="s">
+      <c r="E32" s="75" t="s">
         <v>112</v>
       </c>
       <c r="F32" s="59"/>
@@ -2820,14 +2820,14 @@
       <c r="S32" s="52"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B33" s="83"/>
+      <c r="B33" s="90"/>
       <c r="C33" s="40" t="s">
         <v>49</v>
       </c>
       <c r="D33" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="E33" s="103" t="s">
+      <c r="E33" s="75" t="s">
         <v>113</v>
       </c>
       <c r="F33" s="59"/>
@@ -2846,14 +2846,14 @@
       <c r="S33" s="52"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B34" s="83"/>
+      <c r="B34" s="90"/>
       <c r="C34" s="40" t="s">
         <v>50</v>
       </c>
       <c r="D34" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="E34" s="103" t="s">
+      <c r="E34" s="75" t="s">
         <v>114</v>
       </c>
       <c r="F34" s="59"/>
@@ -2872,14 +2872,14 @@
       <c r="S34" s="52"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B35" s="83"/>
+      <c r="B35" s="90"/>
       <c r="C35" s="42" t="s">
         <v>51</v>
       </c>
       <c r="D35" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="E35" s="103" t="s">
+      <c r="E35" s="75" t="s">
         <v>115</v>
       </c>
       <c r="F35" s="59"/>
@@ -2898,14 +2898,14 @@
       <c r="S35" s="52"/>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B36" s="83"/>
+      <c r="B36" s="90"/>
       <c r="C36" s="40" t="s">
         <v>52</v>
       </c>
       <c r="D36" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="E36" s="103" t="s">
+      <c r="E36" s="75" t="s">
         <v>116</v>
       </c>
       <c r="F36" s="59"/>
@@ -2924,14 +2924,14 @@
       <c r="S36" s="52"/>
     </row>
     <row r="37" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="84"/>
+      <c r="B37" s="91"/>
       <c r="C37" s="43" t="s">
         <v>53</v>
       </c>
       <c r="D37" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="E37" s="104" t="s">
+      <c r="E37" s="76" t="s">
         <v>117</v>
       </c>
       <c r="F37" s="61"/>
@@ -2950,7 +2950,7 @@
       <c r="S37" s="49"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="S1AOELBYt6/XOWTpFRCtaOTetcdUEQLpNxTcriTyQqR7MCbDkGBv0zTywWR1wQrjkN8mQJoTbNbjQqwEyUQd3g==" saltValue="nCuj8+GXpxALTSwhCjkizg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="s+hl0Vzd7+p1ANZVrL5V6iw1tCB3E6BwfsYE74OiIITXcrVxqzvouMaW7AslgnmzCq4Ael3ziKafUcD7PtZtiA==" saltValue="Y4H5WUiY43VaZf6q2SHsSQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="B22:B37"/>

</xml_diff>